<commit_message>
added Punkte for Notenvorschlag
</commit_message>
<xml_diff>
--- a/Notenschlüssel.xlsx
+++ b/Notenschlüssel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\PycharmProjects\Moodle_Sync_Aggregate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B258CF3-C650-4215-B18B-7A4D02744CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82032857-4825-4C6B-B805-CDB03B60EA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{EDA89615-F761-4C9F-B9FE-A5872EDD622D}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -213,7 +212,10 @@
     <t>*</t>
   </si>
   <si>
-    <t>5er</t>
+    <t>GEK2</t>
+  </si>
+  <si>
+    <t>Gkü</t>
   </si>
 </sst>
 </file>
@@ -366,7 +368,13 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -387,9 +395,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F3BE93F-82CC-41AD-B74B-4EBDF489ED86}" name="Tabelle1" displayName="Tabelle1" ref="A1:K22" totalsRowShown="0">
-  <autoFilter ref="A1:K22" xr:uid="{3F3BE93F-82CC-41AD-B74B-4EBDF489ED86}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F3BE93F-82CC-41AD-B74B-4EBDF489ED86}" name="Tabelle1" displayName="Tabelle1" ref="A1:J22" totalsRowShown="0">
+  <autoFilter ref="A1:J22" xr:uid="{3F3BE93F-82CC-41AD-B74B-4EBDF489ED86}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{6417D67E-66A9-46BD-860E-9809C486FD64}" name="Name"/>
     <tableColumn id="2" xr3:uid="{846584E1-DF4B-4069-8EA0-1D83E71E8731}" name="GK1"/>
     <tableColumn id="3" xr3:uid="{8A3A9A68-180B-4895-9E29-DFA04AE4046F}" name="GK2"/>
@@ -398,13 +406,12 @@
     <tableColumn id="6" xr3:uid="{97F74720-4E62-454D-99DB-D8A22E2E0F74}" name="EK2"/>
     <tableColumn id="7" xr3:uid="{DA00DE8C-42B5-4FB3-AC6A-A068FC026980}" name="Note"/>
     <tableColumn id="10" xr3:uid="{52349B72-221B-48DC-99D4-E57341E3C43B}" name="P"/>
-    <tableColumn id="8" xr3:uid="{D57F3716-307C-4079-9D83-18C5DD1D0F4C}" name="Punkte" dataDxfId="1">
-      <calculatedColumnFormula>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{D57F3716-307C-4079-9D83-18C5DD1D0F4C}" name="Punkte" dataDxfId="0">
+      <calculatedColumnFormula array="1">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{03EB3164-F433-407E-9EB3-7C38B9588421}" name="Notenvorschlag" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{03EB3164-F433-407E-9EB3-7C38B9588421}" name="Notenvorschlag" dataDxfId="3">
       <calculatedColumnFormula array="1">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle1[[#This Row],[GK1]] &amp; Tabelle1[[#This Row],[GK2]] &amp; Tabelle1[[#This Row],[GEK1]])))&gt;0,$M$2,Tabelle1[[#This Row],[Punkte]]&gt;=$P$6,$M$6,Tabelle1[[#This Row],[Punkte]]&gt;=$P$5,$M$5,Tabelle1[[#This Row],[Punkte]]&gt;=$P$4,$M$4,Tabelle1[[#This Row],[Punkte]]&gt;=$P$3,$M$3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D4B7C206-2C16-492D-B8B8-55C2F442768F}" name="5er"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -427,6 +434,50 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4F3432F2-2BAF-4F2E-8D6A-A622EB9AA298}" name="K"/>
     <tableColumn id="2" xr3:uid="{1839566A-7A66-4694-90A9-8EA7A67538B6}" name="P"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EF3FF647-180F-4548-836E-B17833035440}" name="Tabelle15" displayName="Tabelle15" ref="A24:I45" totalsRowShown="0">
+  <autoFilter ref="A24:I45" xr:uid="{EF3FF647-180F-4548-836E-B17833035440}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{AAEC7D55-351D-4487-9D3A-64080EE647A4}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{7FD9B135-15B1-4CEF-85DB-EF0054B72AF6}" name="GK1"/>
+    <tableColumn id="3" xr3:uid="{D6115417-C7A3-4702-AD98-51F7D2BCF2EE}" name="GK2"/>
+    <tableColumn id="4" xr3:uid="{5FCA3F97-CD98-4686-ADA2-BD0017B742AF}" name="GEK1"/>
+    <tableColumn id="5" xr3:uid="{4791A52E-B59E-4D26-AF4E-5C748420A6A6}" name="GEK2"/>
+    <tableColumn id="6" xr3:uid="{89007827-E04D-4171-A7DA-81ECC01088F0}" name="EK1"/>
+    <tableColumn id="7" xr3:uid="{3F2BD56D-8603-4269-85AF-91FC845AF502}" name="EK2"/>
+    <tableColumn id="9" xr3:uid="{BEE58C1D-117F-46A3-9C5D-07939CD24AB3}" name="Punkte" dataDxfId="1">
+      <calculatedColumnFormula>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{7CD060A1-A2A5-41C7-B58C-21F5CA6763D7}" name="Notenvorschlag" dataDxfId="2">
+      <calculatedColumnFormula array="1">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D74187D6-C3D1-46AB-AB32-7C069281D708}" name="Tabelle26" displayName="Tabelle26" ref="U24:V27" totalsRowShown="0">
+  <autoFilter ref="U24:V27" xr:uid="{D74187D6-C3D1-46AB-AB32-7C069281D708}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{B6815D12-AEF9-4BED-BF6D-F08DE0E3B4B2}" name="K"/>
+    <tableColumn id="2" xr3:uid="{5182C360-F653-4FAE-A4C8-768E1D5CC630}" name="Anzahl"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C02F06C6-4815-4A41-8486-490730949FF7}" name="Tabelle37" displayName="Tabelle37" ref="R24:S29" totalsRowShown="0">
+  <autoFilter ref="R24:S29" xr:uid="{C02F06C6-4815-4A41-8486-490730949FF7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{8442F57F-7781-473D-A083-603A9E6F2EAE}" name="K"/>
+    <tableColumn id="2" xr3:uid="{1FE13D65-2E59-4A67-8FC6-998EA3839C4F}" name="P"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -729,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7478BD59-11A1-4DF2-AFF0-88B70B2B4E2F}">
-  <dimension ref="A1:AA22"/>
+  <dimension ref="A1:AB45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,21 +794,22 @@
     <col min="5" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="11" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.140625" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.140625" customWidth="1"/>
+    <col min="18" max="18" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" customWidth="1"/>
+    <col min="20" max="20" width="4.140625" customWidth="1"/>
     <col min="21" max="21" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -788,9 +840,6 @@
       <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" t="s">
-        <v>51</v>
-      </c>
       <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
@@ -816,7 +865,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -841,8 +890,8 @@
       <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="I2">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I2" cm="1">
+        <f t="array" ref="I2">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>-2</v>
       </c>
       <c r="J2" cm="1">
@@ -868,7 +917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -893,8 +942,8 @@
       <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="I3">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I3" cm="1">
+        <f t="array" ref="I3">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>0</v>
       </c>
       <c r="J3" cm="1">
@@ -931,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -956,8 +1005,8 @@
       <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="I4">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I4" cm="1">
+        <f t="array" ref="I4">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>3</v>
       </c>
       <c r="J4" cm="1">
@@ -989,8 +1038,18 @@
       <c r="V4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB4" cm="1">
+        <f t="array" ref="AB4">SUMPRODUCT(--EXACT(Z4:AA4, "ü"))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1015,8 +1074,8 @@
       <c r="H5">
         <v>-3</v>
       </c>
-      <c r="I5">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I5" cm="1">
+        <f t="array" ref="I5">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>-3</v>
       </c>
       <c r="J5" cm="1">
@@ -1043,7 +1102,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1068,8 +1127,8 @@
       <c r="H6">
         <v>-2</v>
       </c>
-      <c r="I6">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I6" cm="1">
+        <f t="array" ref="I6">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>-2</v>
       </c>
       <c r="J6" cm="1">
@@ -1090,7 +1149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1115,17 +1174,17 @@
       <c r="H7">
         <v>-1</v>
       </c>
-      <c r="I7">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I7" cm="1">
+        <f t="array" ref="I7">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>-1</v>
       </c>
       <c r="J7" cm="1">
         <f t="array" ref="J7">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle1[[#This Row],[GK1]] &amp; Tabelle1[[#This Row],[GK2]] &amp; Tabelle1[[#This Row],[GEK1]])))&gt;0,$M$2,Tabelle1[[#This Row],[Punkte]]&gt;=$P$6,$M$6,Tabelle1[[#This Row],[Punkte]]&gt;=$P$5,$M$5,Tabelle1[[#This Row],[Punkte]]&gt;=$P$4,$M$4,Tabelle1[[#This Row],[Punkte]]&gt;=$P$3,$M$3)</f>
         <v>3</v>
       </c>
-      <c r="N7" s="13"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1150,8 +1209,8 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I8" cm="1">
+        <f t="array" ref="I8">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>0</v>
       </c>
       <c r="J8" cm="1">
@@ -1159,7 +1218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1184,8 +1243,8 @@
       <c r="H9">
         <v>-1</v>
       </c>
-      <c r="I9">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I9" cm="1">
+        <f t="array" ref="I9">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>-1</v>
       </c>
       <c r="J9" cm="1">
@@ -1193,7 +1252,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1218,8 +1277,8 @@
       <c r="H10">
         <v>-1</v>
       </c>
-      <c r="I10">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I10" cm="1">
+        <f t="array" ref="I10">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>-1</v>
       </c>
       <c r="J10" cm="1">
@@ -1227,7 +1286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1252,8 +1311,8 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I11" cm="1">
+        <f t="array" ref="I11">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>1</v>
       </c>
       <c r="J11" cm="1">
@@ -1261,7 +1320,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1286,8 +1345,8 @@
       <c r="H12">
         <v>2</v>
       </c>
-      <c r="I12">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I12" cm="1">
+        <f t="array" ref="I12">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>2</v>
       </c>
       <c r="J12" cm="1">
@@ -1295,7 +1354,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1320,8 +1379,8 @@
       <c r="H13">
         <v>2</v>
       </c>
-      <c r="I13">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I13" cm="1">
+        <f t="array" ref="I13">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>2</v>
       </c>
       <c r="J13" cm="1">
@@ -1329,7 +1388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1354,8 +1413,8 @@
       <c r="H14">
         <v>2</v>
       </c>
-      <c r="I14">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I14" cm="1">
+        <f t="array" ref="I14">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>2</v>
       </c>
       <c r="J14" cm="1">
@@ -1363,7 +1422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1388,8 +1447,8 @@
       <c r="H15">
         <v>2</v>
       </c>
-      <c r="I15">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I15" cm="1">
+        <f t="array" ref="I15">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>2</v>
       </c>
       <c r="J15" cm="1">
@@ -1397,7 +1456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1422,17 +1481,17 @@
       <c r="H16">
         <v>2</v>
       </c>
-      <c r="I16">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I16" cm="1">
+        <f t="array" ref="I16">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>2</v>
       </c>
       <c r="J16" cm="1">
         <f t="array" ref="J16">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle1[[#This Row],[GK1]] &amp; Tabelle1[[#This Row],[GK2]] &amp; Tabelle1[[#This Row],[GEK1]])))&gt;0,$M$2,Tabelle1[[#This Row],[Punkte]]&gt;=$P$6,$M$6,Tabelle1[[#This Row],[Punkte]]&gt;=$P$5,$M$5,Tabelle1[[#This Row],[Punkte]]&gt;=$P$4,$M$4,Tabelle1[[#This Row],[Punkte]]&gt;=$P$3,$M$3)</f>
         <v>2</v>
       </c>
-      <c r="AA16" s="14"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="Z16" s="14"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1457,8 +1516,8 @@
       <c r="H17">
         <v>4</v>
       </c>
-      <c r="I17">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I17" cm="1">
+        <f t="array" ref="I17">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>4</v>
       </c>
       <c r="J17" cm="1">
@@ -1466,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1491,16 +1550,16 @@
       <c r="H18">
         <v>5</v>
       </c>
-      <c r="I18">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
-        <v>5</v>
+      <c r="I18" cm="1">
+        <f t="array" ref="I18">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
+        <v>4</v>
       </c>
       <c r="J18" cm="1">
         <f t="array" ref="J18">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle1[[#This Row],[GK1]] &amp; Tabelle1[[#This Row],[GK2]] &amp; Tabelle1[[#This Row],[GEK1]])))&gt;0,$M$2,Tabelle1[[#This Row],[Punkte]]&gt;=$P$6,$M$6,Tabelle1[[#This Row],[Punkte]]&gt;=$P$5,$M$5,Tabelle1[[#This Row],[Punkte]]&gt;=$P$4,$M$4,Tabelle1[[#This Row],[Punkte]]&gt;=$P$3,$M$3)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1525,8 +1584,8 @@
       <c r="H19">
         <v>4</v>
       </c>
-      <c r="I19">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I19" cm="1">
+        <f t="array" ref="I19">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>4</v>
       </c>
       <c r="J19" cm="1">
@@ -1534,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1559,16 +1618,16 @@
       <c r="H20">
         <v>4</v>
       </c>
-      <c r="I20">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
-        <v>4</v>
+      <c r="I20" cm="1">
+        <f t="array" ref="I20">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
+        <v>3</v>
       </c>
       <c r="J20" cm="1">
         <f t="array" ref="J20">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle1[[#This Row],[GK1]] &amp; Tabelle1[[#This Row],[GK2]] &amp; Tabelle1[[#This Row],[GEK1]])))&gt;0,$M$2,Tabelle1[[#This Row],[Punkte]]&gt;=$P$6,$M$6,Tabelle1[[#This Row],[Punkte]]&gt;=$P$5,$M$5,Tabelle1[[#This Row],[Punkte]]&gt;=$P$4,$M$4,Tabelle1[[#This Row],[Punkte]]&gt;=$P$3,$M$3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1593,8 +1652,8 @@
       <c r="H21">
         <v>4</v>
       </c>
-      <c r="I21">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I21" cm="1">
+        <f t="array" ref="I21">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>4</v>
       </c>
       <c r="J21" cm="1">
@@ -1602,7 +1661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1627,8 +1686,8 @@
       <c r="H22">
         <v>6</v>
       </c>
-      <c r="I22">
-        <f>COUNTIF(Tabelle1[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Gkü")*-1+COUNTIF(Tabelle1[[#This Row],[GEK1]],"Ekü")+COUNTIF(Tabelle1[[#This Row],[GEK1]],"EKv")*2+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle1[[#This Row],[EK1]:[EK2]],"v")*2</f>
+      <c r="I22" cm="1">
+        <f t="array" ref="I22">SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GK1]:[GK2]],"ü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"GKü"))*-1+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[GEK1]],"EKv"))*2+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"ü"))+SUMPRODUCT(--EXACT(Tabelle1[[#This Row],[EK1]:[EK2]],"v"))*2</f>
         <v>6</v>
       </c>
       <c r="J22" cm="1">
@@ -1636,8 +1695,853 @@
         <v>1</v>
       </c>
     </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" t="s">
+        <v>15</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R24" t="s">
+        <v>12</v>
+      </c>
+      <c r="S24" t="s">
+        <v>26</v>
+      </c>
+      <c r="U24" t="s">
+        <v>12</v>
+      </c>
+      <c r="V24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>-2</v>
+      </c>
+      <c r="I25" cm="1">
+        <f t="array" ref="I25">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>5</v>
+      </c>
+      <c r="M25" s="5">
+        <v>5</v>
+      </c>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="7"/>
+      <c r="R25" t="s">
+        <v>8</v>
+      </c>
+      <c r="S25">
+        <v>-1</v>
+      </c>
+      <c r="U25" t="s">
+        <v>31</v>
+      </c>
+      <c r="V25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>0</v>
+      </c>
+      <c r="I26" cm="1">
+        <f t="array" ref="I26">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>5</v>
+      </c>
+      <c r="M26" s="5">
+        <v>4</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O26" s="6">
+        <f>V25+Tabelle26[[#This Row],[Anzahl]]</f>
+        <v>4</v>
+      </c>
+      <c r="P26" s="12">
+        <f>O26*-1</f>
+        <v>-4</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>50</v>
+      </c>
+      <c r="R26" t="s">
+        <v>7</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="U26" t="s">
+        <v>32</v>
+      </c>
+      <c r="V26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>3</v>
+      </c>
+      <c r="I27" cm="1">
+        <f t="array" ref="I27">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>5</v>
+      </c>
+      <c r="M27" s="5">
+        <v>3</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O27" s="6">
+        <v>3</v>
+      </c>
+      <c r="P27" s="7">
+        <f>O27-O26</f>
+        <v>-1</v>
+      </c>
+      <c r="R27" t="s">
+        <v>9</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="U27" t="s">
+        <v>33</v>
+      </c>
+      <c r="V27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>-3</v>
+      </c>
+      <c r="I28" cm="1">
+        <f t="array" ref="I28">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>4</v>
+      </c>
+      <c r="M28" s="5">
+        <v>2</v>
+      </c>
+      <c r="N28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O28" s="6">
+        <v>3</v>
+      </c>
+      <c r="P28" s="7">
+        <f>O28</f>
+        <v>3</v>
+      </c>
+      <c r="R28" t="s">
+        <v>10</v>
+      </c>
+      <c r="S28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>-2</v>
+      </c>
+      <c r="I29" cm="1">
+        <f t="array" ref="I29">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>4</v>
+      </c>
+      <c r="M29" s="8">
+        <v>1</v>
+      </c>
+      <c r="N29" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="O29" s="9">
+        <v>3</v>
+      </c>
+      <c r="P29" s="10">
+        <f>O29*2</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>-1</v>
+      </c>
+      <c r="I30" cm="1">
+        <f t="array" ref="I30">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>3</v>
+      </c>
+      <c r="M30" s="13"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>0</v>
+      </c>
+      <c r="I31" cm="1">
+        <f t="array" ref="I31">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>-1</v>
+      </c>
+      <c r="I32" cm="1">
+        <f t="array" ref="I32">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>-1</v>
+      </c>
+      <c r="I33" cm="1">
+        <f t="array" ref="I33">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>1</v>
+      </c>
+      <c r="I34" cm="1">
+        <f t="array" ref="I34">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>2</v>
+      </c>
+      <c r="I35" cm="1">
+        <f t="array" ref="I35">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>2</v>
+      </c>
+      <c r="I36" cm="1">
+        <f t="array" ref="I36">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>2</v>
+      </c>
+      <c r="I37" cm="1">
+        <f t="array" ref="I37">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>2</v>
+      </c>
+      <c r="I38" cm="1">
+        <f t="array" ref="I38">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>2</v>
+      </c>
+      <c r="I39" cm="1">
+        <f t="array" ref="I39">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>4</v>
+      </c>
+      <c r="I40" cm="1">
+        <f t="array" ref="I40">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>5</v>
+      </c>
+      <c r="I41" cm="1">
+        <f t="array" ref="I41">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>4</v>
+      </c>
+      <c r="I42" cm="1">
+        <f t="array" ref="I42">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" t="s">
+        <v>21</v>
+      </c>
+      <c r="H43">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>4</v>
+      </c>
+      <c r="I43" cm="1">
+        <f t="array" ref="I43">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>6</v>
+      </c>
+      <c r="I44" cm="1">
+        <f t="array" ref="I44">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45">
+        <f>COUNTIF(Tabelle15[[#This Row],[GK1]:[GK2]],"ü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Gkü")*-1+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"Ekü")+COUNTIF(Tabelle15[[#This Row],[GEK1]:[GEK2]],"EKv")*2+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"ü")+COUNTIF(Tabelle15[[#This Row],[EK1]:[EK2]],"v")*2</f>
+        <v>8</v>
+      </c>
+      <c r="I45" cm="1">
+        <f t="array" ref="I45">_xlfn.IFS(SUMPRODUCT(--ISNUMBER(FIND({"n";"-"},Tabelle15[[#This Row],[GK1]] &amp; Tabelle15[[#This Row],[GK2]] &amp; Tabelle15[[#This Row],[GEK1]] &amp; Tabelle15[[#This Row],[GEK2]])))&gt;0,$M$25,Tabelle15[[#This Row],[Punkte]]&gt;=$P$29,$M$29,Tabelle15[[#This Row],[Punkte]]&gt;=$P$28,$M$28,Tabelle15[[#This Row],[Punkte]]&gt;=$P$27,$M$27,Tabelle15[[#This Row],[Punkte]]&gt;=$P$26,$M$26)</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G22">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M6">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J22">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M25:M29">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1649,7 +2553,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M6">
+  <conditionalFormatting sqref="I25:I45">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1661,8 +2565,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:K22">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="I25">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1673,12 +2577,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H25:H45">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>